<commit_message>
Updated data into cost estimation excel sheet.
</commit_message>
<xml_diff>
--- a/cost_estimation.xlsx
+++ b/cost_estimation.xlsx
@@ -1,27 +1,141 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538360\Documents\github\GDP-1-project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1330CDC0-AB1E-4317-A921-99B872C8FF71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+  <si>
+    <t>Work Breakdown Structure Categories</t>
+  </si>
+  <si>
+    <t>Total Team Cost</t>
+  </si>
+  <si>
+    <t>No. of Hours per week</t>
+  </si>
+  <si>
+    <t>Total cost per week</t>
+  </si>
+  <si>
+    <t>Total cost for three sprints</t>
+  </si>
+  <si>
+    <t>Designation</t>
+  </si>
+  <si>
+    <t>$/hour</t>
+  </si>
+  <si>
+    <t>Planning</t>
+  </si>
+  <si>
+    <t>Designing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    UI Design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Synthesis of Design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Implementation Iteration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Early release and contract finalization</t>
+  </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Application Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    PWA Implementation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Android/IOS implementation</t>
+  </si>
+  <si>
+    <t>Monitoring and controlling</t>
+  </si>
+  <si>
+    <t>Closing</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Initiating</t>
+  </si>
+  <si>
+    <t>Team Leader</t>
+  </si>
+  <si>
+    <t>Project Manager</t>
+  </si>
+  <si>
+    <t>Full Stack Developer</t>
+  </si>
+  <si>
+    <t>UI Developer</t>
+  </si>
+  <si>
+    <t>Database Engineer</t>
+  </si>
+  <si>
+    <t>Front end Developer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                                                             Team-01, Section-02 , Dr. Denise Case</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -37,7 +151,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +159,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +468,338 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="33.453125" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" customWidth="1"/>
+    <col min="3" max="3" width="19.36328125" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" customWidth="1"/>
+    <col min="5" max="5" width="23.7265625" customWidth="1"/>
+    <col min="8" max="8" width="19.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2">
+        <v>350</v>
+      </c>
+      <c r="C5" s="1">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2">
+        <f>B5*C5</f>
+        <v>3150</v>
+      </c>
+      <c r="E5" s="6">
+        <f>$D5*6</f>
+        <v>18900</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2">
+        <v>350</v>
+      </c>
+      <c r="C6" s="1">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2">
+        <f>B6*C6</f>
+        <v>4200</v>
+      </c>
+      <c r="E6" s="2">
+        <f>D6*6</f>
+        <v>25200</v>
+      </c>
+      <c r="H6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2">
+        <v>350</v>
+      </c>
+      <c r="C7" s="1">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2">
+        <f>B7*C7</f>
+        <v>3850</v>
+      </c>
+      <c r="E7" s="2">
+        <f>D7*6</f>
+        <v>23100</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
+        <f>--D2</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2">
+        <v>350</v>
+      </c>
+      <c r="C12" s="1">
+        <v>12</v>
+      </c>
+      <c r="D12" s="2">
+        <f>B12*C12</f>
+        <v>4200</v>
+      </c>
+      <c r="E12" s="2">
+        <f>D12*6</f>
+        <v>25200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="2">
+        <v>350</v>
+      </c>
+      <c r="C16" s="1">
+        <v>11</v>
+      </c>
+      <c r="D16" s="2">
+        <f>B16*C16</f>
+        <v>3850</v>
+      </c>
+      <c r="E16" s="2">
+        <f>D16*6</f>
+        <v>23100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="2">
+        <v>350</v>
+      </c>
+      <c r="C17" s="1">
+        <v>10</v>
+      </c>
+      <c r="D17" s="2">
+        <f>B17*C17</f>
+        <v>3500</v>
+      </c>
+      <c r="E17" s="2">
+        <f>D17*6</f>
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="2">
+        <f>E5+E6+E7+E12+E16+E17</f>
+        <v>136500</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:XFD1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cost estimation of the application
</commit_message>
<xml_diff>
--- a/cost_estimation.xlsx
+++ b/cost_estimation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538360\Documents\github\GDP-1-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s538099\Desktop\GDP-1-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1330CDC0-AB1E-4317-A921-99B872C8FF71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82435B38-37BF-4840-A21B-6AFBE35ADFC0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -472,7 +472,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>